<commit_message>
Update results.xlsx with deception quadrant prediction scores for both LSTM & CNN models
</commit_message>
<xml_diff>
--- a/documents/results.xlsx
+++ b/documents/results.xlsx
@@ -459,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1534,8 +1534,17 @@
       <c r="M28" s="5" t="n">
         <v>0.932</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N28" s="5" t="n">
+        <v>0.9438</v>
+      </c>
+      <c r="O28" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" s="5" t="n">
+        <v>0.971</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>23</v>
       </c>
@@ -1574,6 +1583,15 @@
       </c>
       <c r="M29" s="5" t="n">
         <v>0.8971</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <v>0.9703</v>
+      </c>
+      <c r="O29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>0.9849</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +2877,7 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update results.xlsx for neural networks for messy data
</commit_message>
<xml_diff>
--- a/documents/results.xlsx
+++ b/documents/results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="61">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Lexical Features (LIWC) </t>
   </si>
   <si>
-    <t xml:space="preserve">Neural Networks (After data cleaning)</t>
+    <t xml:space="preserve">Neural Networks</t>
   </si>
   <si>
     <t xml:space="preserve">LSTM</t>
@@ -102,9 +102,6 @@
   <si>
     <t xml:space="preserve">RF gamemove + RF reasoning + RF Rapport + RF ShareInformation = OneHotEncoding
 3 Dense Layers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neural Networks</t>
   </si>
   <si>
     <t xml:space="preserve">0.7581 (acc)</t>
@@ -459,8 +456,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1635,8 +1632,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2663,7 +2660,107 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>0.7351</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>0.8469</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>0.7812</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>0.9969</v>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>0.8752</v>
+      </c>
+      <c r="H28" s="5" t="n">
+        <v>0.6321</v>
+      </c>
+      <c r="I28" s="5" t="n">
+        <v>0.7863</v>
+      </c>
+      <c r="J28" s="5" t="n">
+        <v>0.7003</v>
+      </c>
+      <c r="K28" s="5" t="n">
+        <v>0.6442</v>
+      </c>
+      <c r="L28" s="5" t="n">
+        <v>0.5795</v>
+      </c>
+      <c r="M28" s="5" t="n">
+        <v>0.6084</v>
+      </c>
+      <c r="N28" s="5" t="n">
+        <v>0.9476</v>
+      </c>
+      <c r="O28" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" s="5" t="n">
+        <v>0.9731</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0.7333</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>0.8458</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>0.8058</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>0.8921</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>0.6321</v>
+      </c>
+      <c r="I29" s="5" t="n">
+        <v>0.9594</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <v>0.7614</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>0.5833</v>
+      </c>
+      <c r="M29" s="5" t="n">
+        <v>0.6031</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <v>0.9476</v>
+      </c>
+      <c r="O29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>0.9731</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,7 +2776,7 @@
         <v>0.398</v>
       </c>
       <c r="P37" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2720,7 +2817,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -2742,115 +2839,115 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2889,7 +2986,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2911,34 +3008,34 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5.35598</v>
@@ -2967,7 +3064,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3.54195</v>
@@ -2996,7 +3093,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.2273</v>

</xml_diff>

<commit_message>
random forests pipeline edit
</commit_message>
<xml_diff>
--- a/documents/results.xlsx
+++ b/documents/results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="246">
   <si>
     <t>Model</t>
   </si>
@@ -834,12 +834,15 @@
   <si>
     <t>Weighted by Rand normal (sklearn)</t>
   </si>
+  <si>
+    <t>Gaussian Naïve Bayes + OHE + 3 dense layers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -879,6 +882,13 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -912,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -961,6 +971,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,13 +1322,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R345"/>
+  <dimension ref="A1:R409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B250" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A228" sqref="A228"/>
-      <selection pane="bottomRight" activeCell="I153" sqref="I153"/>
+      <selection pane="bottomRight" activeCell="H274" sqref="H274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8872,13 +8885,13 @@
         <v>0.92849999999999999</v>
       </c>
       <c r="N233">
-        <v>0.94550000000000001</v>
+        <v>0.94410000000000005</v>
       </c>
       <c r="O233">
         <v>1</v>
       </c>
       <c r="P233">
-        <v>0.9718</v>
+        <v>0.97089999999999999</v>
       </c>
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
@@ -8886,2248 +8899,2602 @@
         <v>177</v>
       </c>
       <c r="H234">
-        <v>0.49965300000000001</v>
+        <v>6.8400000000000002E-2</v>
       </c>
       <c r="I234">
-        <v>0.49948399999999998</v>
+        <v>0.5</v>
       </c>
       <c r="J234" s="1">
-        <v>0.49312</v>
+        <v>0.12</v>
       </c>
       <c r="N234">
-        <v>0.472943</v>
+        <v>2.81E-2</v>
       </c>
       <c r="O234">
-        <v>0.49976700000000002</v>
+        <v>0.5</v>
       </c>
       <c r="P234">
-        <v>0.485985</v>
-      </c>
-    </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5.33E-2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="H235">
+        <v>65</v>
+      </c>
+      <c r="H235" s="1">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I235">
+      <c r="I235" s="1">
         <v>1</v>
       </c>
       <c r="J235" s="1">
         <v>0.92849999999999999</v>
       </c>
-      <c r="N235">
-        <v>0.94550000000000001</v>
-      </c>
-      <c r="O235">
-        <v>1</v>
-      </c>
-      <c r="P235">
-        <v>0.9718</v>
-      </c>
-    </row>
-    <row r="236" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="H236">
-        <v>0.43359700000000001</v>
-      </c>
-      <c r="I236">
+      <c r="N235" s="1">
+        <v>0.94410000000000005</v>
+      </c>
+      <c r="O235" s="1">
+        <v>1</v>
+      </c>
+      <c r="P235" s="1">
+        <v>0.97089999999999999</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A236" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="H236" s="1">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="I236" s="1">
         <v>0.5</v>
       </c>
       <c r="J236" s="1">
-        <v>0.46443699999999999</v>
-      </c>
-      <c r="N236">
-        <v>0.49086000000000002</v>
-      </c>
-      <c r="O236">
-        <v>0.49185000000000001</v>
-      </c>
-      <c r="P236">
-        <v>0.49129</v>
-      </c>
-    </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+      <c r="N236" s="1">
+        <v>2.81E-2</v>
+      </c>
+      <c r="O236" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P236" s="1">
+        <v>5.33E-2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H237">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I237">
-        <v>1</v>
-      </c>
-      <c r="J237" s="1">
-        <v>0.92849999999999999</v>
-      </c>
-      <c r="N237">
-        <v>0.94550000000000001</v>
-      </c>
-      <c r="O237">
-        <v>1</v>
-      </c>
-      <c r="P237">
-        <v>0.9718</v>
-      </c>
-    </row>
-    <row r="238" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="H238">
-        <v>0.56642999999999999</v>
-      </c>
-      <c r="I238">
-        <v>0.50019999999999998</v>
-      </c>
-      <c r="J238" s="1">
-        <v>0.117788</v>
-      </c>
-      <c r="N238">
-        <v>0.47295500000000001</v>
-      </c>
-      <c r="O238">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A239" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A240" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A241" s="24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A242" s="24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A244" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A246" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A248" s="24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A250" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A252" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="9"/>
+    </row>
+    <row r="268" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H269" s="1">
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="I269" s="1">
+        <v>1</v>
+      </c>
+      <c r="J269" s="1">
+        <v>0.92710000000000004</v>
+      </c>
+      <c r="N269" s="1">
+        <v>0.95240000000000002</v>
+      </c>
+      <c r="O269" s="1">
+        <v>1</v>
+      </c>
+      <c r="P269" s="1">
+        <v>0.97540000000000004</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H270" s="1">
+        <v>6.7720000000000002E-2</v>
+      </c>
+      <c r="I270" s="1">
         <v>0.5</v>
       </c>
-      <c r="P238">
-        <v>0.48610100000000001</v>
-      </c>
-    </row>
-    <row r="239" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="9"/>
-    </row>
-    <row r="240" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H241">
-        <v>0.98</v>
-      </c>
-      <c r="I241">
-        <v>0.86</v>
-      </c>
-      <c r="J241" s="1">
-        <v>0.91</v>
-      </c>
-      <c r="N241">
-        <v>1</v>
-      </c>
-      <c r="O241">
-        <v>0.95</v>
-      </c>
-      <c r="P241">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A242" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="H242">
-        <v>0.51063999999999998</v>
-      </c>
-      <c r="I242">
-        <v>0.50104400000000004</v>
-      </c>
-      <c r="J242" s="1">
-        <v>0.47427999999999998</v>
-      </c>
-      <c r="N242">
-        <v>0.47289999999999999</v>
-      </c>
-      <c r="O242">
+      <c r="J270" s="1">
+        <v>0.11928</v>
+      </c>
+      <c r="N270" s="1">
+        <v>2.3740000000000001E-2</v>
+      </c>
+      <c r="O270" s="1">
         <v>0.5</v>
       </c>
-      <c r="P242">
-        <v>0.48610100000000001</v>
-      </c>
-    </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A243" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="H243">
-        <v>0.82</v>
-      </c>
-      <c r="I243">
-        <v>0.8</v>
-      </c>
-      <c r="J243" s="1">
-        <v>0.81</v>
-      </c>
-      <c r="N243">
-        <v>0.91</v>
-      </c>
-      <c r="O243">
-        <v>0.91</v>
-      </c>
-      <c r="P243">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="244" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A244" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="H244">
-        <v>0.52729999999999999</v>
-      </c>
-      <c r="I244">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="J244" s="1">
-        <v>0.52428900000000001</v>
-      </c>
-      <c r="N244">
-        <v>0.51158499999999996</v>
-      </c>
-      <c r="O244">
-        <v>0.50997000000000003</v>
-      </c>
-      <c r="P244">
-        <v>0.51049999999999995</v>
-      </c>
-    </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A245" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H245">
-        <v>0.75</v>
-      </c>
-      <c r="I245">
-        <v>0.76</v>
-      </c>
-      <c r="J245" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="N245">
-        <v>0.9</v>
-      </c>
-      <c r="O245">
-        <v>0.9</v>
-      </c>
-      <c r="P245">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="246" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A246" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="H246">
-        <v>0.51670000000000005</v>
-      </c>
-      <c r="I246">
-        <v>0.51490000000000002</v>
-      </c>
-      <c r="J246" s="1">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="N246">
-        <v>0.49696000000000001</v>
-      </c>
-      <c r="O246">
-        <v>0.49697999999999998</v>
-      </c>
-      <c r="P246">
-        <v>0.49697000000000002</v>
-      </c>
-    </row>
-    <row r="247" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="9"/>
-    </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A248" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A249" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H249">
-        <v>0.92730000000000001</v>
-      </c>
-      <c r="I249">
-        <v>1</v>
-      </c>
-      <c r="J249" s="1">
-        <v>0.86560000000000004</v>
-      </c>
-      <c r="N249">
-        <v>0.97909999999999997</v>
-      </c>
-      <c r="O249">
-        <v>1</v>
-      </c>
-      <c r="P249">
-        <v>0.95940000000000003</v>
-      </c>
-    </row>
-    <row r="250" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="H250" s="21">
-        <v>0.47590500000000002</v>
-      </c>
-      <c r="I250" s="21">
-        <v>0.45176899999999998</v>
-      </c>
-      <c r="J250" s="21">
-        <v>0.42346400000000001</v>
-      </c>
-      <c r="N250" s="21">
-        <v>0.49375999999999998</v>
-      </c>
-      <c r="O250" s="21">
-        <v>0.4869</v>
-      </c>
-      <c r="P250" s="21">
-        <v>0.48514000000000002</v>
-      </c>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A251" s="6" t="s">
+      <c r="P270" s="1">
+        <v>4.5339999999999998E-2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H251">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="I251">
-        <v>1</v>
-      </c>
-      <c r="J251" s="1">
-        <v>0.92310000000000003</v>
-      </c>
-      <c r="N251">
-        <v>0.9456</v>
-      </c>
-      <c r="O251">
-        <v>1</v>
-      </c>
-      <c r="P251">
-        <v>0.9718</v>
-      </c>
-    </row>
-    <row r="252" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A252" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H252">
-        <v>6.5083500000000002E-2</v>
-      </c>
-      <c r="I252">
-        <v>0.5</v>
-      </c>
-      <c r="J252" s="1">
-        <v>0.115175</v>
-      </c>
-      <c r="N252">
-        <v>2.4846E-2</v>
-      </c>
-      <c r="O252">
-        <v>0.5</v>
-      </c>
-      <c r="P252">
-        <v>4.7329999999999997E-2</v>
-      </c>
-    </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A253" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H253">
-        <v>7.0800000000000002E-2</v>
-      </c>
-      <c r="I253">
-        <v>0.5</v>
-      </c>
-      <c r="J253" s="1">
-        <v>0.12403</v>
-      </c>
-      <c r="N253">
-        <v>0.49685499999999999</v>
-      </c>
-      <c r="O253">
-        <v>0.48395460000000001</v>
-      </c>
-      <c r="P253">
-        <v>0.40194999999999997</v>
-      </c>
-    </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A254" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H254">
-        <v>0.8619</v>
-      </c>
-      <c r="I254">
-        <v>1</v>
-      </c>
-      <c r="J254" s="1">
-        <v>0.92530000000000001</v>
-      </c>
-      <c r="N254">
-        <v>0.94850000000000001</v>
-      </c>
-      <c r="O254">
-        <v>1</v>
-      </c>
-      <c r="P254">
-        <v>0.97330000000000005</v>
-      </c>
-    </row>
-    <row r="255" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A255" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="H255">
-        <v>6.8821400000000005E-2</v>
-      </c>
-      <c r="I255">
-        <v>0.5</v>
-      </c>
-      <c r="J255" s="1">
-        <v>0.12098</v>
-      </c>
-      <c r="N255">
-        <v>2.5725499999999998E-2</v>
-      </c>
-      <c r="O255">
-        <v>0.5</v>
-      </c>
-      <c r="P255">
-        <v>4.8933499999999998E-2</v>
-      </c>
-    </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A256" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H256">
-        <v>0.8619</v>
-      </c>
-      <c r="I256">
-        <v>1</v>
-      </c>
-      <c r="J256" s="1">
-        <v>0.92530000000000001</v>
-      </c>
-      <c r="N256">
-        <v>0.94769999999999999</v>
-      </c>
-      <c r="O256">
-        <v>1</v>
-      </c>
-      <c r="P256">
-        <v>0.97289999999999999</v>
-      </c>
-    </row>
-    <row r="257" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A257" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="H257">
-        <v>6.8821450000000006E-2</v>
-      </c>
-      <c r="I257">
-        <v>0.5</v>
-      </c>
-      <c r="J257" s="1">
-        <v>0.120989</v>
-      </c>
-      <c r="N257">
-        <v>6.8821450000000006E-2</v>
-      </c>
-      <c r="O257">
-        <v>0.5</v>
-      </c>
-      <c r="P257">
-        <v>0.120989</v>
-      </c>
-    </row>
-    <row r="258" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A258" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H258">
-        <v>0.87009999999999998</v>
-      </c>
-      <c r="I258">
-        <v>1</v>
-      </c>
-      <c r="J258" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N258">
-        <v>0.95230000000000004</v>
-      </c>
-      <c r="O258">
-        <v>1</v>
-      </c>
-      <c r="P258">
-        <v>0.97529999999999994</v>
-      </c>
-    </row>
-    <row r="259" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A259" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="H259">
-        <v>6.4643799000000002E-2</v>
-      </c>
-      <c r="I259">
-        <v>0.5</v>
-      </c>
-      <c r="J259" s="1">
-        <v>0.114485</v>
-      </c>
-      <c r="N259">
-        <v>6.4640000000000003E-2</v>
-      </c>
-      <c r="O259">
-        <v>0.5</v>
-      </c>
-      <c r="P259">
-        <v>0.11448</v>
-      </c>
-    </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A260" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="H260">
-        <v>0.87009999999999998</v>
-      </c>
-      <c r="I260">
-        <v>1</v>
-      </c>
-      <c r="J260" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N260">
-        <v>0.95230000000000004</v>
-      </c>
-      <c r="O260">
-        <v>1</v>
-      </c>
-      <c r="P260">
-        <v>0.97529999999999994</v>
-      </c>
-    </row>
-    <row r="261" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A261" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="H261">
-        <v>6.4640000000000003E-2</v>
-      </c>
-      <c r="I261">
-        <v>0.5</v>
-      </c>
-      <c r="J261" s="1">
-        <v>0.11448</v>
-      </c>
-      <c r="N261">
-        <v>2.3966500000000002E-2</v>
-      </c>
-      <c r="O261">
-        <v>0.5</v>
-      </c>
-      <c r="P261">
-        <v>4.5740000000000003E-2</v>
-      </c>
-    </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A262" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H262">
-        <v>0.86260000000000003</v>
-      </c>
-      <c r="I262">
-        <v>1</v>
-      </c>
-      <c r="J262" s="1">
-        <v>0.92569999999999997</v>
-      </c>
-      <c r="N262">
-        <v>0.94930000000000003</v>
-      </c>
-      <c r="O262">
-        <v>1</v>
-      </c>
-      <c r="P262">
-        <v>0.9738</v>
-      </c>
-    </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A263" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H263">
-        <v>6.8821450000000006E-2</v>
-      </c>
-      <c r="I263">
-        <v>0.5</v>
-      </c>
-      <c r="J263" s="1">
-        <v>0.120989</v>
-      </c>
-      <c r="N263">
-        <v>2.5284999999999998E-2</v>
-      </c>
-      <c r="O263">
-        <v>0.5</v>
-      </c>
-      <c r="P263">
-        <v>4.8136999999999999E-2</v>
-      </c>
-    </row>
-    <row r="264" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="9"/>
-    </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A265" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="266" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="H266" s="25">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="I266" s="25">
-        <v>1.5E-3</v>
-      </c>
-      <c r="J266" s="25">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="N266" s="25">
-        <v>0.9506</v>
-      </c>
-      <c r="O266" s="25">
-        <v>1</v>
-      </c>
-      <c r="P266" s="25">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="267" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="H267" s="21">
-        <v>6.4420000000000005E-2</v>
-      </c>
-      <c r="I267" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="J267" s="21">
-        <v>0.11414000000000001</v>
-      </c>
-      <c r="N267" s="21">
-        <v>2.4625999999999999E-2</v>
-      </c>
-      <c r="O267" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P267" s="21">
-        <v>4.6940000000000003E-2</v>
-      </c>
-    </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A268" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H268">
-        <v>0.95879999999999999</v>
-      </c>
-      <c r="I268">
-        <v>0.19689999999999999</v>
-      </c>
-      <c r="J268" s="1">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="N268">
-        <v>0.94869999999999999</v>
-      </c>
-      <c r="O268">
-        <v>0.3957</v>
-      </c>
-      <c r="P268">
-        <v>0.55510000000000004</v>
-      </c>
-    </row>
-    <row r="269" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A269" s="9" t="s">
+    </row>
+    <row r="272" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="H269">
-        <v>6.4423900000000006E-2</v>
-      </c>
-      <c r="I269">
-        <v>0.5</v>
-      </c>
-      <c r="J269" s="1">
-        <v>0.11414000000000001</v>
-      </c>
-      <c r="N269">
-        <v>2.4625999999999999E-2</v>
-      </c>
-      <c r="O269">
-        <v>0.5</v>
-      </c>
-      <c r="P269">
-        <v>4.6940000000000003E-2</v>
-      </c>
-    </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A270" s="9" t="s">
+      <c r="H272" s="1">
+        <v>0.87270000000000003</v>
+      </c>
+      <c r="I272" s="1">
+        <v>1</v>
+      </c>
+      <c r="J272" s="1">
+        <v>0.93159999999999998</v>
+      </c>
+      <c r="N272" s="1">
+        <v>0.9476</v>
+      </c>
+      <c r="O272" s="1">
+        <v>1</v>
+      </c>
+      <c r="P272" s="1">
+        <v>0.9728</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H270" s="1">
-        <v>0.87009999999999998</v>
-      </c>
-      <c r="I270" s="1">
-        <v>1</v>
-      </c>
-      <c r="J270" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N270">
-        <v>0.95050000000000001</v>
-      </c>
-      <c r="O270">
-        <v>0.79090000000000005</v>
-      </c>
-      <c r="P270">
-        <v>0.86250000000000004</v>
-      </c>
-    </row>
-    <row r="271" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A271" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="H271" s="21">
-        <v>6.4640000000000003E-2</v>
-      </c>
-      <c r="I271" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="J271" s="21">
-        <v>0.11448</v>
-      </c>
-      <c r="N271" s="21">
-        <v>2.4625999999999999E-2</v>
-      </c>
-      <c r="O271" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P271" s="21">
-        <v>4.6940000000000003E-2</v>
-      </c>
-    </row>
-    <row r="272" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A272" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="H272" s="1">
-        <v>0.92349999999999999</v>
-      </c>
-      <c r="I272" s="1">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="J272" s="1">
-        <v>0.51119999999999999</v>
-      </c>
-      <c r="N272" s="1">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="O272" s="1">
-        <v>0.58720000000000006</v>
-      </c>
-      <c r="P272" s="1">
-        <v>0.72240000000000004</v>
-      </c>
-    </row>
-    <row r="273" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A273" s="9" t="s">
-        <v>222</v>
-      </c>
       <c r="H273" s="1">
-        <v>6.4423900000000006E-2</v>
+        <v>6.3539999999999999E-2</v>
       </c>
       <c r="I273" s="1">
         <v>0.5</v>
       </c>
       <c r="J273" s="1">
-        <v>0.11414000000000001</v>
+        <v>0.113</v>
       </c>
       <c r="N273" s="1">
-        <v>2.4625999999999999E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="O273" s="1">
         <v>0.5</v>
       </c>
       <c r="P273" s="1">
-        <v>4.6940000000000003E-2</v>
+        <v>4.9299999999999997E-2</v>
       </c>
     </row>
     <row r="274" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A275" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A277" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="H274" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I274" s="1">
-        <v>1</v>
-      </c>
-      <c r="J274" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N274" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O274" s="1">
-        <v>1</v>
-      </c>
-      <c r="P274" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="275" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A275" s="9" t="s">
+    </row>
+    <row r="278" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A278" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="H275" s="1">
+    </row>
+    <row r="279" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A280" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A282" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A284" s="24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A286" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A288" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A294" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A296" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="9"/>
+    </row>
+    <row r="304" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A305" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H305">
+        <v>0.98</v>
+      </c>
+      <c r="I305">
+        <v>0.86</v>
+      </c>
+      <c r="J305" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="N305">
+        <v>1</v>
+      </c>
+      <c r="O305">
+        <v>0.95</v>
+      </c>
+      <c r="P305">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A306" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H306">
+        <v>0.51063999999999998</v>
+      </c>
+      <c r="I306">
+        <v>0.50104400000000004</v>
+      </c>
+      <c r="J306" s="1">
+        <v>0.47427999999999998</v>
+      </c>
+      <c r="N306">
+        <v>0.47289999999999999</v>
+      </c>
+      <c r="O306">
+        <v>0.5</v>
+      </c>
+      <c r="P306">
+        <v>0.48610100000000001</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A307" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H307">
+        <v>0.82</v>
+      </c>
+      <c r="I307">
+        <v>0.8</v>
+      </c>
+      <c r="J307" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="N307">
+        <v>0.91</v>
+      </c>
+      <c r="O307">
+        <v>0.91</v>
+      </c>
+      <c r="P307">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="308" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A308" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="H308">
+        <v>0.52729999999999999</v>
+      </c>
+      <c r="I308">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="J308" s="1">
+        <v>0.52428900000000001</v>
+      </c>
+      <c r="N308">
+        <v>0.51158499999999996</v>
+      </c>
+      <c r="O308">
+        <v>0.50997000000000003</v>
+      </c>
+      <c r="P308">
+        <v>0.51049999999999995</v>
+      </c>
+    </row>
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A309" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H309">
+        <v>0.75</v>
+      </c>
+      <c r="I309">
+        <v>0.76</v>
+      </c>
+      <c r="J309" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="N309">
+        <v>0.9</v>
+      </c>
+      <c r="O309">
+        <v>0.9</v>
+      </c>
+      <c r="P309">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A310" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H310">
+        <v>0.51670000000000005</v>
+      </c>
+      <c r="I310">
+        <v>0.51490000000000002</v>
+      </c>
+      <c r="J310" s="1">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="N310">
+        <v>0.49696000000000001</v>
+      </c>
+      <c r="O310">
+        <v>0.49697999999999998</v>
+      </c>
+      <c r="P310">
+        <v>0.49697000000000002</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="9"/>
+    </row>
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A312" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A313" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H313">
+        <v>0.92730000000000001</v>
+      </c>
+      <c r="I313">
+        <v>1</v>
+      </c>
+      <c r="J313" s="1">
+        <v>0.86560000000000004</v>
+      </c>
+      <c r="N313">
+        <v>0.97909999999999997</v>
+      </c>
+      <c r="O313">
+        <v>1</v>
+      </c>
+      <c r="P313">
+        <v>0.95940000000000003</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="H314" s="21">
+        <v>0.47590500000000002</v>
+      </c>
+      <c r="I314" s="21">
+        <v>0.45176899999999998</v>
+      </c>
+      <c r="J314" s="21">
+        <v>0.42346400000000001</v>
+      </c>
+      <c r="N314" s="21">
+        <v>0.49375999999999998</v>
+      </c>
+      <c r="O314" s="21">
+        <v>0.4869</v>
+      </c>
+      <c r="P314" s="21">
+        <v>0.48514000000000002</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A315" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H315">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="I315">
+        <v>1</v>
+      </c>
+      <c r="J315" s="1">
+        <v>0.92310000000000003</v>
+      </c>
+      <c r="N315">
+        <v>0.9456</v>
+      </c>
+      <c r="O315">
+        <v>1</v>
+      </c>
+      <c r="P315">
+        <v>0.9718</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A316" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H316">
+        <v>6.5083500000000002E-2</v>
+      </c>
+      <c r="I316">
+        <v>0.5</v>
+      </c>
+      <c r="J316" s="1">
+        <v>0.115175</v>
+      </c>
+      <c r="N316">
+        <v>2.4846E-2</v>
+      </c>
+      <c r="O316">
+        <v>0.5</v>
+      </c>
+      <c r="P316">
+        <v>4.7329999999999997E-2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A317" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H317">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="I317">
+        <v>0.5</v>
+      </c>
+      <c r="J317" s="1">
+        <v>0.12403</v>
+      </c>
+      <c r="N317">
+        <v>0.49685499999999999</v>
+      </c>
+      <c r="O317">
+        <v>0.48395460000000001</v>
+      </c>
+      <c r="P317">
+        <v>0.40194999999999997</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A318" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H318">
+        <v>0.8619</v>
+      </c>
+      <c r="I318">
+        <v>1</v>
+      </c>
+      <c r="J318" s="1">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="N318">
+        <v>0.94850000000000001</v>
+      </c>
+      <c r="O318">
+        <v>1</v>
+      </c>
+      <c r="P318">
+        <v>0.97330000000000005</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A319" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H319">
+        <v>6.8821400000000005E-2</v>
+      </c>
+      <c r="I319">
+        <v>0.5</v>
+      </c>
+      <c r="J319" s="1">
+        <v>0.12098</v>
+      </c>
+      <c r="N319">
+        <v>2.5725499999999998E-2</v>
+      </c>
+      <c r="O319">
+        <v>0.5</v>
+      </c>
+      <c r="P319">
+        <v>4.8933499999999998E-2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A320" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H320">
+        <v>0.8619</v>
+      </c>
+      <c r="I320">
+        <v>1</v>
+      </c>
+      <c r="J320" s="1">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="N320">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="O320">
+        <v>1</v>
+      </c>
+      <c r="P320">
+        <v>0.97289999999999999</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A321" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H321">
+        <v>6.8821450000000006E-2</v>
+      </c>
+      <c r="I321">
+        <v>0.5</v>
+      </c>
+      <c r="J321" s="1">
+        <v>0.120989</v>
+      </c>
+      <c r="N321">
+        <v>6.8821450000000006E-2</v>
+      </c>
+      <c r="O321">
+        <v>0.5</v>
+      </c>
+      <c r="P321">
+        <v>0.120989</v>
+      </c>
+    </row>
+    <row r="322" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A322" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H322">
+        <v>0.87009999999999998</v>
+      </c>
+      <c r="I322">
+        <v>1</v>
+      </c>
+      <c r="J322" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N322">
+        <v>0.95230000000000004</v>
+      </c>
+      <c r="O322">
+        <v>1</v>
+      </c>
+      <c r="P322">
+        <v>0.97529999999999994</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A323" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H323">
+        <v>6.4643799000000002E-2</v>
+      </c>
+      <c r="I323">
+        <v>0.5</v>
+      </c>
+      <c r="J323" s="1">
+        <v>0.114485</v>
+      </c>
+      <c r="N323">
+        <v>6.4640000000000003E-2</v>
+      </c>
+      <c r="O323">
+        <v>0.5</v>
+      </c>
+      <c r="P323">
+        <v>0.11448</v>
+      </c>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A324" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H324">
+        <v>0.87009999999999998</v>
+      </c>
+      <c r="I324">
+        <v>1</v>
+      </c>
+      <c r="J324" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N324">
+        <v>0.95230000000000004</v>
+      </c>
+      <c r="O324">
+        <v>1</v>
+      </c>
+      <c r="P324">
+        <v>0.97529999999999994</v>
+      </c>
+    </row>
+    <row r="325" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A325" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H325">
+        <v>6.4640000000000003E-2</v>
+      </c>
+      <c r="I325">
+        <v>0.5</v>
+      </c>
+      <c r="J325" s="1">
+        <v>0.11448</v>
+      </c>
+      <c r="N325">
+        <v>2.3966500000000002E-2</v>
+      </c>
+      <c r="O325">
+        <v>0.5</v>
+      </c>
+      <c r="P325">
+        <v>4.5740000000000003E-2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A326" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H326">
+        <v>0.86260000000000003</v>
+      </c>
+      <c r="I326">
+        <v>1</v>
+      </c>
+      <c r="J326" s="1">
+        <v>0.92569999999999997</v>
+      </c>
+      <c r="N326">
+        <v>0.94930000000000003</v>
+      </c>
+      <c r="O326">
+        <v>1</v>
+      </c>
+      <c r="P326">
+        <v>0.9738</v>
+      </c>
+    </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A327" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H327">
+        <v>6.8821450000000006E-2</v>
+      </c>
+      <c r="I327">
+        <v>0.5</v>
+      </c>
+      <c r="J327" s="1">
+        <v>0.120989</v>
+      </c>
+      <c r="N327">
+        <v>2.5284999999999998E-2</v>
+      </c>
+      <c r="O327">
+        <v>0.5</v>
+      </c>
+      <c r="P327">
+        <v>4.8136999999999999E-2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="9"/>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A329" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="330" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="H330" s="25">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="I330" s="25">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J330" s="25">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="N330" s="25">
+        <v>0.9506</v>
+      </c>
+      <c r="O330" s="25">
+        <v>1</v>
+      </c>
+      <c r="P330" s="25">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="H331" s="21">
+        <v>6.4420000000000005E-2</v>
+      </c>
+      <c r="I331" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J331" s="21">
+        <v>0.11414000000000001</v>
+      </c>
+      <c r="N331" s="21">
+        <v>2.4625999999999999E-2</v>
+      </c>
+      <c r="O331" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P331" s="21">
+        <v>4.6940000000000003E-2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A332" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H332">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="I332">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="J332" s="1">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="N332">
+        <v>0.94869999999999999</v>
+      </c>
+      <c r="O332">
+        <v>0.3957</v>
+      </c>
+      <c r="P332">
+        <v>0.55510000000000004</v>
+      </c>
+    </row>
+    <row r="333" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A333" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H333">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I275" s="1">
+      <c r="I333">
         <v>0.5</v>
       </c>
-      <c r="J275" s="1">
+      <c r="J333" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N275" s="1">
+      <c r="N333">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O275" s="1">
+      <c r="O333">
         <v>0.5</v>
       </c>
-      <c r="P275" s="1">
+      <c r="P333">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="9" t="s">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A334" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H334" s="1">
+        <v>0.87009999999999998</v>
+      </c>
+      <c r="I334" s="1">
+        <v>1</v>
+      </c>
+      <c r="J334" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N334">
+        <v>0.95050000000000001</v>
+      </c>
+      <c r="O334">
+        <v>0.79090000000000005</v>
+      </c>
+      <c r="P334">
+        <v>0.86250000000000004</v>
+      </c>
+    </row>
+    <row r="335" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A335" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="H335" s="21">
+        <v>6.4640000000000003E-2</v>
+      </c>
+      <c r="I335" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J335" s="21">
+        <v>0.11448</v>
+      </c>
+      <c r="N335" s="21">
+        <v>2.4625999999999999E-2</v>
+      </c>
+      <c r="O335" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P335" s="21">
+        <v>4.6940000000000003E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A336" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H336" s="1">
+        <v>0.92349999999999999</v>
+      </c>
+      <c r="I336" s="1">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="J336" s="1">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="N336" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="O336" s="1">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="P336" s="1">
+        <v>0.72240000000000004</v>
+      </c>
+    </row>
+    <row r="337" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A337" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H337" s="1">
+        <v>6.4423900000000006E-2</v>
+      </c>
+      <c r="I337" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J337" s="1">
+        <v>0.11414000000000001</v>
+      </c>
+      <c r="N337" s="1">
+        <v>2.4625999999999999E-2</v>
+      </c>
+      <c r="O337" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P337" s="1">
+        <v>4.6940000000000003E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A338" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H338" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I338" s="1">
+        <v>1</v>
+      </c>
+      <c r="J338" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N338" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O338" s="1">
+        <v>1</v>
+      </c>
+      <c r="P338" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A339" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="H339" s="1">
+        <v>6.4423900000000006E-2</v>
+      </c>
+      <c r="I339" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J339" s="1">
+        <v>0.11414000000000001</v>
+      </c>
+      <c r="N339" s="1">
+        <v>2.4625999999999999E-2</v>
+      </c>
+      <c r="O339" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P339" s="1">
+        <v>4.6940000000000003E-2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H276" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I276" s="1">
-        <v>1</v>
-      </c>
-      <c r="J276" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N276" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O276" s="1">
-        <v>1</v>
-      </c>
-      <c r="P276" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="277" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A277" s="22" t="s">
+      <c r="H340" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I340" s="1">
+        <v>1</v>
+      </c>
+      <c r="J340" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N340" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O340" s="1">
+        <v>1</v>
+      </c>
+      <c r="P340" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="341" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A341" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="H277" s="21">
+      <c r="H341" s="21">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I277" s="21">
+      <c r="I341" s="21">
         <v>0.5</v>
       </c>
-      <c r="J277" s="21">
+      <c r="J341" s="21">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N277" s="21">
+      <c r="N341" s="21">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O277" s="21">
+      <c r="O341" s="21">
         <v>0.5</v>
       </c>
-      <c r="P277" s="21">
+      <c r="P341" s="21">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A278" s="9" t="s">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A342" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H278" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I278" s="1">
-        <v>1</v>
-      </c>
-      <c r="J278" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N278">
+      <c r="H342" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I342" s="1">
+        <v>1</v>
+      </c>
+      <c r="J342" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N342">
         <v>0.95069999999999999</v>
       </c>
-      <c r="O278" s="1">
+      <c r="O342" s="1">
         <v>0.89880000000000004</v>
       </c>
-      <c r="P278">
+      <c r="P342">
         <v>0.92359999999999998</v>
       </c>
     </row>
-    <row r="279" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A279" s="9" t="s">
+    <row r="343" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A343" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="H279" s="1">
+      <c r="H343" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I279" s="1">
+      <c r="I343" s="1">
         <v>0.5</v>
       </c>
-      <c r="J279" s="1">
+      <c r="J343" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N279" s="1">
+      <c r="N343" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O279" s="1">
+      <c r="O343" s="1">
         <v>0.5</v>
       </c>
-      <c r="P279" s="1">
+      <c r="P343" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="9" t="s">
+    <row r="344" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H280" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I280" s="1">
-        <v>1</v>
-      </c>
-      <c r="J280" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N280" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O280" s="1">
-        <v>1</v>
-      </c>
-      <c r="P280" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="281" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A281" s="22" t="s">
+      <c r="H344" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I344" s="1">
+        <v>1</v>
+      </c>
+      <c r="J344" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N344" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O344" s="1">
+        <v>1</v>
+      </c>
+      <c r="P344" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A345" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="H281" s="21">
+      <c r="H345" s="21">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I281" s="21">
+      <c r="I345" s="21">
         <v>0.5</v>
       </c>
-      <c r="J281" s="21">
+      <c r="J345" s="21">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N281" s="21">
+      <c r="N345" s="21">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O281" s="21">
+      <c r="O345" s="21">
         <v>0.5</v>
       </c>
-      <c r="P281" s="21">
+      <c r="P345" s="21">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="282" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="9" t="s">
+    <row r="346" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H282" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I282" s="1">
-        <v>1</v>
-      </c>
-      <c r="J282" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N282" s="1">
+      <c r="H346" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I346" s="1">
+        <v>1</v>
+      </c>
+      <c r="J346" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N346" s="1">
         <v>0.95120000000000005</v>
       </c>
-      <c r="O282" s="1">
+      <c r="O346" s="1">
         <v>0.93940000000000001</v>
       </c>
-      <c r="P282" s="1">
+      <c r="P346" s="1">
         <v>0.94479999999999997</v>
       </c>
     </row>
-    <row r="283" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A283" s="9" t="s">
+    <row r="347" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A347" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H283" s="1">
+      <c r="H347" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I283" s="1">
+      <c r="I347" s="1">
         <v>0.5</v>
       </c>
-      <c r="J283" s="1">
+      <c r="J347" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N283" s="1">
+      <c r="N347" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O283" s="1">
+      <c r="O347" s="1">
         <v>0.5</v>
       </c>
-      <c r="P283" s="1">
+      <c r="P347" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="284" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="9" t="s">
+    <row r="348" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="H284" s="1">
+      <c r="H348" s="1">
         <v>0.87809999999999999</v>
       </c>
-      <c r="I284" s="1">
+      <c r="I348" s="1">
         <v>0.79039999999999999</v>
       </c>
-      <c r="J284" s="1">
+      <c r="J348" s="1">
         <v>0.8306</v>
       </c>
-      <c r="N284" s="1">
+      <c r="N348" s="1">
         <v>0.94689999999999996</v>
       </c>
-      <c r="O284" s="1">
+      <c r="O348" s="1">
         <v>0.50129999999999997</v>
       </c>
-      <c r="P284" s="1">
+      <c r="P348" s="1">
         <v>0.65310000000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A285" s="9" t="s">
+    <row r="349" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A349" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="H285" s="1">
+      <c r="H349" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I285" s="1">
+      <c r="I349" s="1">
         <v>0.5</v>
       </c>
-      <c r="J285" s="1">
+      <c r="J349" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N285" s="1">
+      <c r="N349" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O285" s="1">
+      <c r="O349" s="1">
         <v>0.5</v>
       </c>
-      <c r="P285" s="1">
+      <c r="P349" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A286" s="9" t="s">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A350" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H286">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I286">
-        <v>1</v>
-      </c>
-      <c r="J286" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N286">
+      <c r="H350">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I350">
+        <v>1</v>
+      </c>
+      <c r="J350" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N350">
         <v>0.94979999999999998</v>
       </c>
-      <c r="O286">
+      <c r="O350">
         <v>0.57889999999999997</v>
       </c>
-      <c r="P286">
+      <c r="P350">
         <v>0.71809999999999996</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A287" s="9" t="s">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A351" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H287" s="1">
+      <c r="H351" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I287" s="1">
+      <c r="I351" s="1">
         <v>0.5</v>
       </c>
-      <c r="J287" s="1">
+      <c r="J351" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N287">
+      <c r="N351">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O287">
+      <c r="O351">
         <v>0.5</v>
       </c>
-      <c r="P287">
+      <c r="P351">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A288" s="9" t="s">
+    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A352" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="H288">
+      <c r="H352">
         <v>0.91679999999999995</v>
       </c>
-      <c r="I288" s="1">
+      <c r="I352" s="1">
         <v>0.66490000000000005</v>
       </c>
-      <c r="J288" s="1">
+      <c r="J352" s="1">
         <v>0.76900000000000002</v>
       </c>
-      <c r="N288">
-        <v>0.9506</v>
-      </c>
-      <c r="O288">
-        <v>1</v>
-      </c>
-      <c r="P288">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A289" s="22" t="s">
+      <c r="N352">
+        <v>0.9506</v>
+      </c>
+      <c r="O352">
+        <v>1</v>
+      </c>
+      <c r="P352">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="353" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A353" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="B289" s="21"/>
-      <c r="C289" s="21"/>
-      <c r="D289" s="21"/>
-      <c r="E289" s="21"/>
-      <c r="F289" s="21"/>
-      <c r="G289" s="21"/>
-      <c r="H289" s="21">
+      <c r="B353" s="21"/>
+      <c r="C353" s="21"/>
+      <c r="D353" s="21"/>
+      <c r="E353" s="21"/>
+      <c r="F353" s="21"/>
+      <c r="G353" s="21"/>
+      <c r="H353" s="21">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I289" s="21">
+      <c r="I353" s="21">
         <v>0.5</v>
       </c>
-      <c r="J289" s="21">
+      <c r="J353" s="21">
         <v>0.11414000000000001</v>
       </c>
-      <c r="K289" s="21"/>
-      <c r="L289" s="21"/>
-      <c r="M289" s="21"/>
-      <c r="N289" s="21">
+      <c r="K353" s="21"/>
+      <c r="L353" s="21"/>
+      <c r="M353" s="21"/>
+      <c r="N353" s="21">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O289" s="21">
+      <c r="O353" s="21">
         <v>0.5</v>
       </c>
-      <c r="P289" s="21">
+      <c r="P353" s="21">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A290" s="9" t="s">
+    <row r="354" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A354" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="H290" s="1">
+      <c r="H354" s="1">
         <v>0.92269999999999996</v>
       </c>
-      <c r="I290" s="1">
+      <c r="I354" s="1">
         <v>0.71060000000000001</v>
       </c>
-      <c r="J290" s="1">
+      <c r="J354" s="1">
         <v>0.90159999999999996</v>
       </c>
-      <c r="K290" s="1"/>
-      <c r="L290" s="1"/>
-      <c r="M290" s="1"/>
-      <c r="N290" s="1">
+      <c r="K354" s="1"/>
+      <c r="L354" s="1"/>
+      <c r="M354" s="1"/>
+      <c r="N354" s="1">
         <v>0.95269999999999999</v>
       </c>
-      <c r="O290" s="1">
+      <c r="O354" s="1">
         <v>0.49099999999999999</v>
       </c>
-      <c r="P290" s="1">
+      <c r="P354" s="1">
         <v>0.64510000000000001</v>
       </c>
     </row>
-    <row r="291" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A291" s="9" t="s">
+    <row r="355" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A355" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="H291" s="1">
+      <c r="H355" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I291" s="1">
+      <c r="I355" s="1">
         <v>0.5</v>
       </c>
-      <c r="J291" s="1">
+      <c r="J355" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N291" s="1">
+      <c r="N355" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O291" s="1">
+      <c r="O355" s="1">
         <v>0.5</v>
       </c>
-      <c r="P291" s="1">
+      <c r="P355" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="9" t="s">
+    <row r="356" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="H292" s="1">
+      <c r="H356" s="1">
         <v>0.87260000000000004</v>
       </c>
-      <c r="I292" s="1">
+      <c r="I356" s="1">
         <v>0.89259999999999995</v>
       </c>
-      <c r="J292" s="1">
+      <c r="J356" s="1">
         <v>0.88160000000000005</v>
       </c>
-      <c r="N292" s="1">
+      <c r="N356" s="1">
         <v>0.95040000000000002</v>
       </c>
-      <c r="O292" s="1">
+      <c r="O356" s="1">
         <v>0.99590000000000001</v>
       </c>
-      <c r="P292" s="1">
+      <c r="P356" s="1">
         <v>0.97240000000000004</v>
       </c>
     </row>
-    <row r="293" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A293" s="9" t="s">
+    <row r="357" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A357" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="H293" s="1">
+      <c r="H357" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I293" s="1">
+      <c r="I357" s="1">
         <v>0.5</v>
       </c>
-      <c r="J293" s="1">
+      <c r="J357" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N293" s="1">
+      <c r="N357" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O293" s="1">
+      <c r="O357" s="1">
         <v>0.5</v>
       </c>
-      <c r="P293" s="1">
+      <c r="P357" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="H294" s="1">
+    <row r="358" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H358" s="1">
         <v>0.93320000000000003</v>
       </c>
-      <c r="I294" s="1">
+      <c r="I358" s="1">
         <v>0.70130000000000003</v>
       </c>
-      <c r="J294" s="1">
+      <c r="J358" s="1">
         <v>0.79979999999999996</v>
       </c>
-      <c r="N294" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O294" s="1">
-        <v>1</v>
-      </c>
-      <c r="P294" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A295" s="9" t="s">
+      <c r="N358" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O358" s="1">
+        <v>1</v>
+      </c>
+      <c r="P358" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="359" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A359" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H295" s="1">
+      <c r="H359" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I295" s="1">
+      <c r="I359" s="1">
         <v>0.5</v>
       </c>
-      <c r="J295" s="1">
+      <c r="J359" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N295" s="1">
+      <c r="N359" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O295" s="1">
+      <c r="O359" s="1">
         <v>0.5</v>
       </c>
-      <c r="P295" s="1">
+      <c r="P359" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="9" t="s">
+    <row r="360" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="H296" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I296" s="1">
-        <v>1</v>
-      </c>
-      <c r="J296" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N296" s="1">
+      <c r="H360" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I360" s="1">
+        <v>1</v>
+      </c>
+      <c r="J360" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N360" s="1">
         <v>0.95589999999999997</v>
       </c>
-      <c r="O296" s="1">
+      <c r="O360" s="1">
         <v>0.61429999999999996</v>
       </c>
-      <c r="P296" s="1">
+      <c r="P360" s="1">
         <v>0.74619999999999997</v>
       </c>
     </row>
-    <row r="297" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="9" t="s">
+    <row r="361" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="H297" s="1">
+      <c r="H361" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I297" s="1">
+      <c r="I361" s="1">
         <v>0.5</v>
       </c>
-      <c r="J297" s="1">
+      <c r="J361" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N297" s="1">
+      <c r="N361" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O297" s="1">
+      <c r="O361" s="1">
         <v>0.5</v>
       </c>
-      <c r="P297" s="1">
+      <c r="P361" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="9"/>
-    </row>
-    <row r="299" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="11" t="s">
+    <row r="362" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="9"/>
+    </row>
+    <row r="363" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="300" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="9" t="s">
+    <row r="364" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="H300" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I300" s="1">
+      <c r="H364" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I364" s="1">
         <v>0.9163</v>
       </c>
-      <c r="J300" s="1">
+      <c r="J364" s="1">
         <v>0.89180000000000004</v>
       </c>
-      <c r="N300" s="1">
+      <c r="N364" s="1">
         <v>0.95079999999999998</v>
       </c>
-      <c r="O300" s="1">
+      <c r="O364" s="1">
         <v>0.88800000000000001</v>
       </c>
-      <c r="P300" s="1">
+      <c r="P364" s="1">
         <v>0.91769999999999996</v>
       </c>
     </row>
-    <row r="301" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="22" t="s">
+    <row r="365" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="H301" s="21">
+      <c r="H365" s="21">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I301" s="21">
+      <c r="I365" s="21">
         <v>0.5</v>
       </c>
-      <c r="J301" s="21">
+      <c r="J365" s="21">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N301" s="21">
+      <c r="N365" s="21">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O301" s="21">
+      <c r="O365" s="21">
         <v>0.5</v>
       </c>
-      <c r="P301" s="21">
+      <c r="P365" s="21">
         <v>4.69404E-2</v>
       </c>
     </row>
-    <row r="302" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="9" t="s">
+    <row r="366" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H302" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I302" s="1">
-        <v>1</v>
-      </c>
-      <c r="J302" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N302" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O302" s="1">
-        <v>1</v>
-      </c>
-      <c r="P302" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="303" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A303" s="9" t="s">
+      <c r="H366" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I366" s="1">
+        <v>1</v>
+      </c>
+      <c r="J366" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N366" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O366" s="1">
+        <v>1</v>
+      </c>
+      <c r="P366" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A367" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="H303" s="1">
+      <c r="H367" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I303" s="1">
+      <c r="I367" s="1">
         <v>0.5</v>
       </c>
-      <c r="J303" s="1">
+      <c r="J367" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N303" s="1">
+      <c r="N367" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O303" s="1">
+      <c r="O367" s="1">
         <v>0.5</v>
       </c>
-      <c r="P303" s="1">
+      <c r="P367" s="1">
         <v>4.69404E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="9" t="s">
+    <row r="368" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H304" s="1">
+      <c r="H368" s="1">
         <v>0.91979999999999995</v>
       </c>
-      <c r="I304" s="1">
+      <c r="I368" s="1">
         <v>0.68569999999999998</v>
       </c>
-      <c r="J304" s="1">
+      <c r="J368" s="1">
         <v>0.7843</v>
       </c>
-      <c r="N304" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O304" s="1">
-        <v>1</v>
-      </c>
-      <c r="P304" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="305" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A305" s="9" t="s">
+      <c r="N368" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O368" s="1">
+        <v>1</v>
+      </c>
+      <c r="P368" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A369" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="H305" s="1">
+      <c r="H369" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I305" s="1">
+      <c r="I369" s="1">
         <v>0.5</v>
       </c>
-      <c r="J305" s="1">
+      <c r="J369" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N305" s="1">
+      <c r="N369" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O305" s="1">
+      <c r="O369" s="1">
         <v>0.5</v>
       </c>
-      <c r="P305" s="1">
+      <c r="P369" s="1">
         <v>4.69404E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="9" t="s">
+    <row r="370" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H306" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I306" s="1">
-        <v>1</v>
-      </c>
-      <c r="J306" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N306" s="1">
+      <c r="H370" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I370" s="1">
+        <v>1</v>
+      </c>
+      <c r="J370" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N370" s="1">
         <v>0.94989999999999997</v>
       </c>
-      <c r="O306" s="1">
+      <c r="O370" s="1">
         <v>0.9335</v>
       </c>
-      <c r="P306" s="1">
+      <c r="P370" s="1">
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="307" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A307" s="9" t="s">
+    <row r="371" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A371" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H307" s="1">
+      <c r="H371" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I307" s="1">
+      <c r="I371" s="1">
         <v>0.5</v>
       </c>
-      <c r="J307" s="1">
+      <c r="J371" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N307" s="1">
+      <c r="N371" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O307" s="1">
+      <c r="O371" s="1">
         <v>0.5</v>
       </c>
-      <c r="P307" s="1">
+      <c r="P371" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="308" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="9" t="s">
+    <row r="372" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H308" s="1">
+      <c r="H372" s="1">
         <v>0.86960000000000004</v>
       </c>
-      <c r="I308" s="1">
+      <c r="I372" s="1">
         <v>0.94530000000000003</v>
       </c>
-      <c r="J308" s="1">
+      <c r="J372" s="1">
         <v>0.9052</v>
       </c>
-      <c r="N308" s="1">
+      <c r="N372" s="1">
         <v>0.95279999999999998</v>
       </c>
-      <c r="O308" s="1">
-        <v>1</v>
-      </c>
-      <c r="P308" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="309" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A309" s="9" t="s">
+      <c r="O372" s="1">
+        <v>1</v>
+      </c>
+      <c r="P372" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="373" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A373" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="H309" s="1">
+      <c r="H373" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I309" s="1">
+      <c r="I373" s="1">
         <v>0.5</v>
       </c>
-      <c r="J309" s="1">
+      <c r="J373" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N309" s="1">
+      <c r="N373" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O309" s="1">
+      <c r="O373" s="1">
         <v>0.5</v>
       </c>
-      <c r="P309" s="1">
+      <c r="P373" s="1">
         <v>4.69404E-2</v>
       </c>
     </row>
-    <row r="310" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A310" s="9" t="s">
+    <row r="374" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A374" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="H310" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I310" s="1">
-        <v>1</v>
-      </c>
-      <c r="J310" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N310" s="1">
+      <c r="H374" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I374" s="1">
+        <v>1</v>
+      </c>
+      <c r="J374" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N374" s="1">
         <v>0.95089999999999997</v>
       </c>
-      <c r="O310" s="1">
+      <c r="O374" s="1">
         <v>0.97219999999999995</v>
       </c>
-      <c r="P310" s="1">
+      <c r="P374" s="1">
         <v>0.96120000000000005</v>
       </c>
     </row>
-    <row r="311" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A311" s="9" t="s">
+    <row r="375" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A375" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="H311" s="1">
+      <c r="H375" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I311" s="1">
+      <c r="I375" s="1">
         <v>0.5</v>
       </c>
-      <c r="J311" s="1">
+      <c r="J375" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N311" s="1">
+      <c r="N375" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O311" s="1">
+      <c r="O375" s="1">
         <v>0.5</v>
       </c>
-      <c r="P311" s="1">
+      <c r="P375" s="1">
         <v>4.69404E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A312" s="9" t="s">
+    <row r="376" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A376" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="H312" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I312" s="1">
-        <v>1</v>
-      </c>
-      <c r="J312" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N312" s="1">
+      <c r="H376" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I376" s="1">
+        <v>1</v>
+      </c>
+      <c r="J376" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N376" s="1">
         <v>0.95109999999999995</v>
       </c>
-      <c r="O312" s="1">
+      <c r="O376" s="1">
         <v>0.87829999999999997</v>
       </c>
-      <c r="P312" s="1">
+      <c r="P376" s="1">
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="313" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A313" s="9" t="s">
+    <row r="377" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A377" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="H313" s="1">
+      <c r="H377" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I313" s="1">
+      <c r="I377" s="1">
         <v>0.5</v>
       </c>
-      <c r="J313" s="1">
+      <c r="J377" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N313" s="1">
+      <c r="N377" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O313" s="1">
+      <c r="O377" s="1">
         <v>0.5</v>
       </c>
-      <c r="P313" s="1">
+      <c r="P377" s="1">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A314" s="9" t="s">
+    <row r="378" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H314" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I314" s="1">
-        <v>1</v>
-      </c>
-      <c r="J314" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N314" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O314" s="1">
-        <v>1</v>
-      </c>
-      <c r="P314" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="315" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A315" s="9" t="s">
+      <c r="H378" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I378" s="1">
+        <v>1</v>
+      </c>
+      <c r="J378" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N378" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O378" s="1">
+        <v>1</v>
+      </c>
+      <c r="P378" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="379" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A379" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="H315" s="1">
+      <c r="H379" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I315" s="1">
+      <c r="I379" s="1">
         <v>0.5</v>
       </c>
-      <c r="J315" s="1">
+      <c r="J379" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N315" s="1">
+      <c r="N379" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O315" s="1">
+      <c r="O379" s="1">
         <v>0.5</v>
       </c>
-      <c r="P315" s="1">
+      <c r="P379" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="316" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="9" t="s">
+    <row r="380" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H316" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I316" s="1">
-        <v>1</v>
-      </c>
-      <c r="J316" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N316" s="1">
+      <c r="H380" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I380" s="1">
+        <v>1</v>
+      </c>
+      <c r="J380" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N380" s="1">
         <v>0.95069999999999999</v>
       </c>
-      <c r="O316" s="1">
-        <v>1</v>
-      </c>
-      <c r="P316" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="317" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A317" s="9" t="s">
+      <c r="O380" s="1">
+        <v>1</v>
+      </c>
+      <c r="P380" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="381" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A381" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H317" s="1">
+      <c r="H381" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I317" s="1">
+      <c r="I381" s="1">
         <v>0.5</v>
       </c>
-      <c r="J317" s="1">
+      <c r="J381" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N317" s="1">
+      <c r="N381" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O317" s="1">
+      <c r="O381" s="1">
         <v>0.5</v>
       </c>
-      <c r="P317" s="1">
+      <c r="P381" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="318" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A318" s="9" t="s">
+    <row r="382" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="H318" s="1">
+      <c r="H382" s="1">
         <v>0.86870000000000003</v>
       </c>
-      <c r="I318" s="1">
+      <c r="I382" s="1">
         <v>0.40100000000000002</v>
       </c>
-      <c r="J318" s="1">
+      <c r="J382" s="1">
         <v>0.54549999999999998</v>
       </c>
-      <c r="N318" s="1">
+      <c r="N382" s="1">
         <v>0.94779999999999998</v>
       </c>
-      <c r="O318" s="1">
+      <c r="O382" s="1">
         <v>0.67430000000000001</v>
       </c>
-      <c r="P318" s="1">
+      <c r="P382" s="1">
         <v>0.78590000000000004</v>
       </c>
     </row>
-    <row r="319" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A319" s="9" t="s">
+    <row r="383" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A383" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="H319" s="1">
+      <c r="H383" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I319" s="1">
+      <c r="I383" s="1">
         <v>0.5</v>
       </c>
-      <c r="J319" s="1">
+      <c r="J383" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N319" s="1">
+      <c r="N383" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O319" s="1">
+      <c r="O383" s="1">
         <v>0.5</v>
       </c>
-      <c r="P319" s="1">
+      <c r="P383" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="320" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A320" s="9" t="s">
+    <row r="384" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A384" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H320" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I320" s="1">
-        <v>1</v>
-      </c>
-      <c r="J320" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N320" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O320" s="1">
-        <v>1</v>
-      </c>
-      <c r="P320" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="321" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A321" s="9" t="s">
+      <c r="H384" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I384" s="1">
+        <v>1</v>
+      </c>
+      <c r="J384" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N384" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O384" s="1">
+        <v>1</v>
+      </c>
+      <c r="P384" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="385" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A385" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H321" s="1">
+      <c r="H385" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I321" s="1">
+      <c r="I385" s="1">
         <v>0.5</v>
       </c>
-      <c r="J321" s="1">
+      <c r="J385" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N321" s="1">
+      <c r="N385" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O321" s="1">
+      <c r="O385" s="1">
         <v>0.5</v>
       </c>
-      <c r="P321" s="1">
+      <c r="P385" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="322" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="9" t="s">
+    <row r="386" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A386" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="H322" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I322" s="1">
-        <v>1</v>
-      </c>
-      <c r="J322" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N322" s="1">
+      <c r="H386" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I386" s="1">
+        <v>1</v>
+      </c>
+      <c r="J386" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N386" s="1">
         <v>0.95069999999999999</v>
       </c>
-      <c r="O322" s="1">
-        <v>1</v>
-      </c>
-      <c r="P322" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="323" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A323" s="9" t="s">
+      <c r="O386" s="1">
+        <v>1</v>
+      </c>
+      <c r="P386" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="387" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A387" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="H323" s="1">
+      <c r="H387" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I323" s="1">
+      <c r="I387" s="1">
         <v>0.5</v>
       </c>
-      <c r="J323" s="1">
+      <c r="J387" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N323" s="1">
+      <c r="N387" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O323" s="1">
+      <c r="O387" s="1">
         <v>0.5</v>
       </c>
-      <c r="P323" s="1">
+      <c r="P387" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="324" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="9" t="s">
+    <row r="388" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A388" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="H324" s="1">
+      <c r="H388" s="1">
         <v>0.92520000000000002</v>
       </c>
-      <c r="I324" s="1">
+      <c r="I388" s="1">
         <v>0.68859999999999999</v>
       </c>
-      <c r="J324" s="1">
+      <c r="J388" s="1">
         <v>0.78779999999999994</v>
       </c>
-      <c r="N324" s="1">
-        <v>0.9506</v>
-      </c>
-      <c r="O324" s="1">
-        <v>1</v>
-      </c>
-      <c r="P324" s="1">
-        <v>0.97450000000000003</v>
-      </c>
-    </row>
-    <row r="325" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A325" s="9" t="s">
+      <c r="N388" s="1">
+        <v>0.9506</v>
+      </c>
+      <c r="O388" s="1">
+        <v>1</v>
+      </c>
+      <c r="P388" s="1">
+        <v>0.97450000000000003</v>
+      </c>
+    </row>
+    <row r="389" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A389" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="H325" s="1">
+      <c r="H389" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I325" s="1">
+      <c r="I389" s="1">
         <v>0.5</v>
       </c>
-      <c r="J325" s="1">
+      <c r="J389" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N325" s="1">
+      <c r="N389" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O325" s="1">
+      <c r="O389" s="1">
         <v>0.5</v>
       </c>
-      <c r="P325" s="1">
+      <c r="P389" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="326" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="9" t="s">
+    <row r="390" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A390" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="H326" s="1">
-        <v>0.86980000000000002</v>
-      </c>
-      <c r="I326" s="1">
-        <v>1</v>
-      </c>
-      <c r="J326" s="1">
-        <v>0.92989999999999995</v>
-      </c>
-      <c r="N326" s="1">
+      <c r="H390" s="1">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="I390" s="1">
+        <v>1</v>
+      </c>
+      <c r="J390" s="1">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="N390" s="1">
         <v>0.94950000000000001</v>
       </c>
-      <c r="O326" s="1">
+      <c r="O390" s="1">
         <v>0.92779999999999996</v>
       </c>
-      <c r="P326" s="1">
+      <c r="P390" s="1">
         <v>0.93789999999999996</v>
       </c>
     </row>
-    <row r="327" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A327" s="9" t="s">
+    <row r="391" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A391" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="H327" s="1">
+      <c r="H391" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I327" s="1">
+      <c r="I391" s="1">
         <v>0.5</v>
       </c>
-      <c r="J327" s="1">
+      <c r="J391" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N327" s="1">
+      <c r="N391" s="1">
         <v>2.46E-2</v>
       </c>
-      <c r="O327" s="1">
+      <c r="O391" s="1">
         <v>0.5</v>
       </c>
-      <c r="P327" s="1">
+      <c r="P391" s="1">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="328" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="H328" s="1">
+    <row r="392" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A392" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H392" s="1">
         <v>0.95499999999999996</v>
       </c>
-      <c r="I328" s="1">
+      <c r="I392" s="1">
         <v>0.62360000000000004</v>
       </c>
-      <c r="J328" s="1">
+      <c r="J392" s="1">
         <v>0.75219999999999998</v>
       </c>
-      <c r="N328" s="1">
+      <c r="N392" s="1">
         <v>0.89870000000000005</v>
       </c>
-      <c r="O328" s="1">
+      <c r="O392" s="1">
         <v>0.30790000000000001</v>
       </c>
-      <c r="P328" s="1">
+      <c r="P392" s="1">
         <v>0.4551</v>
       </c>
     </row>
-    <row r="329" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A329" s="9" t="s">
+    <row r="393" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A393" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H329" s="1">
+      <c r="H393" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="I329" s="1">
+      <c r="I393" s="1">
         <v>0.5</v>
       </c>
-      <c r="J329" s="1">
+      <c r="J393" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
-      <c r="N329" s="1">
+      <c r="N393" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="O329" s="1">
+      <c r="O393" s="1">
         <v>0.5</v>
       </c>
-      <c r="P329" s="1">
+      <c r="P393" s="1">
         <v>0.11414000000000001</v>
       </c>
     </row>
-    <row r="330" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A330" s="9" t="s">
+    <row r="394" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A394" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="H330" s="1">
+      <c r="H394" s="1">
         <v>0.89870000000000005</v>
       </c>
-      <c r="I330" s="1">
+      <c r="I394" s="1">
         <v>0.60309999999999997</v>
       </c>
-      <c r="J330" s="1">
+      <c r="J394" s="1">
         <v>0.72</v>
       </c>
-      <c r="N330" s="1">
+      <c r="N394" s="1">
         <v>0.94799999999999995</v>
       </c>
-      <c r="O330" s="1">
+      <c r="O394" s="1">
         <v>0.44619999999999999</v>
       </c>
-      <c r="P330" s="1">
+      <c r="P394" s="1">
         <v>0.60370000000000001</v>
       </c>
     </row>
-    <row r="331" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A331" s="9" t="s">
+    <row r="395" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A395" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="H331" s="1">
+      <c r="H395" s="1">
         <v>6.4423900000000006E-2</v>
       </c>
-      <c r="I331" s="1">
+      <c r="I395" s="1">
         <v>0.5</v>
       </c>
-      <c r="J331" s="1">
+      <c r="J395" s="1">
         <v>0.11414000000000001</v>
       </c>
-      <c r="N331" s="1">
+      <c r="N395" s="1">
         <v>2.4625999999999999E-2</v>
       </c>
-      <c r="O331" s="1">
+      <c r="O395" s="1">
         <v>0.5</v>
       </c>
-      <c r="P331" s="1">
+      <c r="P395" s="1">
         <v>4.6940000000000003E-2</v>
       </c>
     </row>
-    <row r="332" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A332" s="9"/>
-    </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A333" s="6"/>
-    </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A334" s="11" t="s">
+    <row r="396" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A396" s="9"/>
+    </row>
+    <row r="397" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A397" s="6"/>
+    </row>
+    <row r="398" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A398" s="11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A335" s="6" t="s">
+    <row r="399" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A399" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H335">
+      <c r="H399">
         <v>0.92730000000000001</v>
       </c>
-      <c r="I335">
-        <v>1</v>
-      </c>
-      <c r="J335" s="1">
+      <c r="I399">
+        <v>1</v>
+      </c>
+      <c r="J399" s="1">
         <v>0.86560000000000004</v>
       </c>
-      <c r="N335">
+      <c r="N399">
         <v>0.86560000000000004</v>
       </c>
-      <c r="O335">
-        <v>1</v>
-      </c>
-      <c r="P335">
+      <c r="O399">
+        <v>1</v>
+      </c>
+      <c r="P399">
         <v>0.92730000000000001</v>
       </c>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A336" s="6" t="s">
+    <row r="400" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A400" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H336">
+      <c r="H400">
         <v>6.8821400000000005E-2</v>
       </c>
-      <c r="I336">
+      <c r="I400">
         <v>0.5</v>
       </c>
-      <c r="J336" s="1">
+      <c r="J400" s="1">
         <v>0.120989</v>
       </c>
-      <c r="N336">
+      <c r="N400">
         <v>6.8820000000000006E-2</v>
       </c>
-      <c r="O336">
+      <c r="O400">
         <v>0.5</v>
       </c>
-      <c r="P336">
+      <c r="P400">
         <v>0.12098</v>
       </c>
     </row>
-    <row r="337" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="11" t="s">
+    <row r="401" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A401" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A338" s="6" t="s">
+    <row r="402" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A402" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H338">
+      <c r="H402">
         <v>0.85750000000000004</v>
       </c>
-      <c r="I338">
+      <c r="I402">
         <v>0.99329999999999996</v>
       </c>
-      <c r="J338" s="1">
+      <c r="J402" s="1">
         <v>0.92</v>
       </c>
-      <c r="N338">
+      <c r="N402">
         <v>0.9456</v>
       </c>
-      <c r="O338">
+      <c r="O402">
         <v>0.99960000000000004</v>
       </c>
-      <c r="P338">
+      <c r="P402">
         <v>0.97160000000000002</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A343" s="11" t="s">
+    <row r="407" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A407" s="11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A344" s="6" t="s">
+    <row r="408" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A408" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H344">
+      <c r="H408">
         <v>0.4</v>
       </c>
-      <c r="I344">
+      <c r="I408">
         <v>0.5</v>
       </c>
-      <c r="J344" s="1">
+      <c r="J408" s="1">
         <v>0.44400000000000001</v>
       </c>
-      <c r="N344">
+      <c r="N408">
         <v>0.50519999999999998</v>
       </c>
-      <c r="O344">
+      <c r="O408">
         <v>0.5202</v>
       </c>
-      <c r="P344">
+      <c r="P408">
         <v>0.4914</v>
       </c>
     </row>
-    <row r="345" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A345" s="6" t="s">
+    <row r="409" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A409" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H345">
+      <c r="H409">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I345">
+      <c r="I409">
         <v>0.61599999999999999</v>
       </c>
-      <c r="J345" s="1">
+      <c r="J409" s="1">
         <v>0.48570000000000002</v>
       </c>
-      <c r="N345">
+      <c r="N409">
         <v>0.5</v>
       </c>
-      <c r="O345">
+      <c r="O409">
         <v>0.34</v>
       </c>
-      <c r="P345">
+      <c r="P409">
         <v>0.40400000000000003</v>
       </c>
     </row>
@@ -11140,7 +11507,7 @@
     <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>